<commit_message>
Massive Changes (Added Printing and Semester)
</commit_message>
<xml_diff>
--- a/exampleDataSubjects.xlsx
+++ b/exampleDataSubjects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TrueLife\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project-management\pm\trial_error1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D47241-17B5-4B15-9355-6AB7DFEF665C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F85B81-F3E1-4B54-A1C5-EA0476819466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
   <si>
     <t>CC223</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>wed</t>
+  </si>
+  <si>
+    <t>305 ICBs</t>
   </si>
 </sst>
 </file>
@@ -604,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +751,7 @@
         <v>0.3125</v>
       </c>
       <c r="B4" s="1">
-        <v>0.47916666666666702</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C4" t="s">
         <v>82</v>
@@ -780,7 +789,7 @@
         <v>0.3125</v>
       </c>
       <c r="B5" s="1">
-        <v>0.52083333333333304</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
@@ -818,7 +827,7 @@
         <v>0.3125</v>
       </c>
       <c r="B6" s="1">
-        <v>0.47916666666666702</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C6" t="s">
         <v>82</v>
@@ -856,7 +865,7 @@
         <v>0.3125</v>
       </c>
       <c r="B7" s="1">
-        <v>0.47916666666666702</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C7" t="s">
         <v>82</v>
@@ -970,7 +979,7 @@
         <v>0.3125</v>
       </c>
       <c r="B10" s="1">
-        <v>0.39583333333333298</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C10" t="s">
         <v>82</v>
@@ -1046,7 +1055,7 @@
         <v>0.3125</v>
       </c>
       <c r="B12" s="1">
-        <v>0.47916666666666702</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C12" t="s">
         <v>80</v>
@@ -1122,7 +1131,7 @@
         <v>0.3125</v>
       </c>
       <c r="B14" s="1">
-        <v>0.39583333333333298</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C14" t="s">
         <v>83</v>
@@ -1198,10 +1207,10 @@
         <v>0.3125</v>
       </c>
       <c r="B16" s="1">
-        <v>0.39583333333333298</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -1231,9 +1240,157 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>